<commit_message>
a few general updates
</commit_message>
<xml_diff>
--- a/resources/volo-data/germimation-experiment.xlsx
+++ b/resources/volo-data/germimation-experiment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anneliserismann/Documents/GitHub/hdbot/resources/volo-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588A8082-A998-8A4E-B079-8BF1C156BEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73B7770-0BB6-7B40-ADE3-6629CD878AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{7911502E-23E9-144C-81EA-E4BDF800C8D6}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="219">
   <si>
     <t>Species</t>
   </si>
@@ -685,6 +686,12 @@
   </si>
   <si>
     <t>3 multiple seedlings</t>
+  </si>
+  <si>
+    <t>26.10.2020_count</t>
+  </si>
+  <si>
+    <t>26.10.2020_comment</t>
   </si>
 </sst>
 </file>
@@ -1052,13 +1059,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2010A8CA-FF1D-184F-B35B-F43FF65F5364}">
-  <dimension ref="A1:X92"/>
+  <dimension ref="A1:Z92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O84" sqref="O84"/>
+      <selection pane="bottomRight" activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1072,7 +1079,7 @@
     <col min="10" max="10" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1145,8 +1152,14 @@
       <c r="X1" s="1" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1208,7 +1221,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1270,7 +1283,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1329,7 +1342,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1385,7 +1398,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1438,7 +1451,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1494,7 +1507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>164</v>
       </c>
@@ -1541,7 +1554,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1597,7 +1610,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1656,7 +1669,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1715,7 +1728,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>206</v>
       </c>
@@ -1771,7 +1784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1824,7 +1837,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -1880,7 +1893,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -1936,7 +1949,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>41</v>
       </c>

</xml_diff>